<commit_message>
added an option to listen to the shoot tiller emergence to emerge nodals
</commit_message>
<xml_diff>
--- a/simulations/scene/inputs/Scenarios_25-08-05.xlsx
+++ b/simulations/scene/inputs/Scenarios_25-08-05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TIGERA~1\AppData\Local\Temp\scp45613\home\torisuten\package\Wheat-BRIDGES\simulations\scene\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EE786A-5E05-47F1-A1F2-EEE0E593597D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118031E0-7B9A-4D61-8585-F17E5544E57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2998" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="597">
   <si>
     <t>input_file</t>
   </si>
@@ -1819,6 +1819,12 @@
   </si>
   <si>
     <t>Before</t>
+  </si>
+  <si>
+    <t>synchronize_adventitious_emergence</t>
+  </si>
+  <si>
+    <t>Tells wether root system should listen to shoot for synchronization of nodal roots emergence</t>
   </si>
 </sst>
 </file>
@@ -2889,13 +2895,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BZ229"/>
+  <dimension ref="A1:BZ230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="O187" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="P189" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U192" sqref="U192"/>
+      <selection pane="bottomRight" activeCell="R220" sqref="R220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32939,11 +32945,11 @@
         <v>0.3</v>
       </c>
       <c r="R206" s="44">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="S206" s="58"/>
       <c r="T206" s="44">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="V206" s="44">
         <v>0.3</v>
@@ -34726,16 +34732,16 @@
         <v>2E-8</v>
       </c>
       <c r="R218" s="44">
-        <f>0.00001 / 2</f>
-        <v>5.0000000000000004E-6</v>
+        <f>0.00001 / 2 / 2</f>
+        <v>2.5000000000000002E-6</v>
       </c>
       <c r="S218" s="44">
         <f>0.00001</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="T218" s="44">
-        <f>0.00001 / 2</f>
-        <v>5.0000000000000004E-6</v>
+        <f>0.00001 / 2 / 2</f>
+        <v>2.5000000000000002E-6</v>
       </c>
       <c r="V218" s="44">
         <v>2E-8</v>
@@ -34943,16 +34949,16 @@
       <c r="O220" s="44"/>
       <c r="P220" s="44"/>
       <c r="R220" s="44">
-        <f>0.00001 /10/4</f>
-        <v>2.5000000000000004E-7</v>
+        <f>0.00001 /10/4 / 2</f>
+        <v>1.2500000000000002E-7</v>
       </c>
       <c r="S220" s="44">
         <f>0.00001 /10/4/2</f>
         <v>1.2500000000000002E-7</v>
       </c>
       <c r="T220" s="44">
-        <f>0.00001 /10/4</f>
-        <v>2.5000000000000004E-7</v>
+        <f>0.00001 /10/4 /2</f>
+        <v>1.2500000000000002E-7</v>
       </c>
       <c r="V220" s="44"/>
       <c r="W220" s="44"/>
@@ -36128,7 +36134,7 @@
         <v>539</v>
       </c>
       <c r="G228" s="44">
-        <f t="shared" ref="G228:BC229" si="27">0.00002 / 14 / 5</f>
+        <f t="shared" ref="G228:BC230" si="27">0.00002 / 14 / 5</f>
         <v>2.8571428571428575E-7</v>
       </c>
       <c r="H228" s="44">
@@ -36316,7 +36322,7 @@
         <v>539</v>
       </c>
       <c r="G229" s="44">
-        <f t="shared" ref="G229:AZ229" si="28">0.00002 / 14 / 5 /10</f>
+        <f t="shared" ref="G229:AZ230" si="28">0.00002 / 14 / 5 /10</f>
         <v>2.8571428571428575E-8</v>
       </c>
       <c r="H229" s="44">
@@ -36484,6 +36490,167 @@
       <c r="BJ229" s="1"/>
       <c r="BK229" s="1"/>
     </row>
+    <row r="230" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="E230" s="30" t="s">
+        <v>596</v>
+      </c>
+      <c r="F230" s="30" t="s">
+        <v>486</v>
+      </c>
+      <c r="G230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="H230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="I230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="J230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="K230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="L230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="M230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="N230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="O230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="P230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="R230" s="44">
+        <v>0</v>
+      </c>
+      <c r="S230" s="58"/>
+      <c r="T230" s="44">
+        <v>0</v>
+      </c>
+      <c r="V230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="W230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="X230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AA230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AB230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AC230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AD230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AE230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AF230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AG230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AH230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AI230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AJ230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AK230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AL230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AM230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AN230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AO230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AP230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AQ230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AR230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AS230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AT230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AU230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AV230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AW230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AX230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AY230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="AZ230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="BA230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="BB230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="BC230" s="44">
+        <v>-1</v>
+      </c>
+      <c r="BD230" s="1"/>
+      <c r="BE230" s="1"/>
+      <c r="BF230" s="1"/>
+      <c r="BG230" s="1"/>
+      <c r="BH230" s="1"/>
+      <c r="BI230" s="1"/>
+      <c r="BJ230" s="1"/>
+      <c r="BK230" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="G211:P211 BC211 V211:X211 R211:T212">
@@ -56878,7 +57045,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BC228:BC229 AA228:AD229 G228:P229 V228:X229 R228:T229">
+  <conditionalFormatting sqref="BC228:BC229 AA228:AD229 R228:T230 G228:P230 V228:X230 AA230:BC230">
     <cfRule type="colorScale" priority="3308">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>